<commit_message>
Generate figures from shiny script to paper format
</commit_message>
<xml_diff>
--- a/tables/network_indices.xlsx
+++ b/tables/network_indices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\message_trade\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jus3\message_trade\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B04966C-6725-4DE9-867D-4D47EBE34534}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88C55D7-B8B4-43D0-B28F-13B4ED41E595}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{372B6620-EE92-499D-9853-4DF8BB550A14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{372B6620-EE92-499D-9853-4DF8BB550A14}"/>
   </bookViews>
   <sheets>
     <sheet name="Network_Index_2020" sheetId="1" r:id="rId1"/>
@@ -23,18 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="32">
   <si>
     <t>Outdegree centrality</t>
   </si>
@@ -124,6 +118,12 @@
   </si>
   <si>
     <t>Imports (EJ)</t>
+  </si>
+  <si>
+    <t>Ethanol</t>
+  </si>
+  <si>
+    <t>Global energy system cost</t>
   </si>
 </sst>
 </file>
@@ -182,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -201,6 +201,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -517,23 +520,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A40B8966-91DF-448A-A8AB-6D833515FB4D}">
-  <dimension ref="B3:H26"/>
+  <dimension ref="B3:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B26"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="6"/>
-    <col min="2" max="2" width="34.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="6"/>
+    <col min="2" max="2" width="34.26953125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="28" style="6" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.1796875" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="28" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="6"/>
+    <col min="9" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
@@ -553,7 +556,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
@@ -573,101 +576,111 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B23" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B24" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B25" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B26" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B27" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B28" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -679,23 +692,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF0B6F6-8AF5-4B15-8E42-218F417DADB6}">
-  <dimension ref="B3:H26"/>
+  <dimension ref="B3:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="6"/>
-    <col min="2" max="2" width="34.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="6"/>
+    <col min="2" max="2" width="34.26953125" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="28" style="6" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.1796875" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="28" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="6"/>
+    <col min="9" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
@@ -715,7 +728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
@@ -735,101 +748,111 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="2:8" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B23" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B24" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B25" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B26" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B27" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B28" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -846,13 +869,13 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="33.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
@@ -872,7 +895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
@@ -892,131 +915,131 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="8"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B16" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" s="8"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B23" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B24" s="8"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B25" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B26" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B27" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B28" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B29" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B30" s="8">
         <v>5</v>
       </c>
@@ -1031,17 +1054,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D22D252F-B740-4CE1-B703-41B9E0EAE28B}">
   <dimension ref="B2:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="33.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1061,7 +1084,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
@@ -1081,131 +1104,131 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="8"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B16" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" s="8"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B23" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B24" s="8"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B25" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B26" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B27" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B28" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B29" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B30" s="8">
         <v>5</v>
       </c>

</xml_diff>